<commit_message>
modified Maze_main.py to have a full screen, deleted unused or repeated asset images
</commit_message>
<xml_diff>
--- a/data/0_maze_log.xlsx
+++ b/data/0_maze_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaodanluo/Desktop/lab_github/MazeGame/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E76E33-11D5-7E44-8F0A-3E6FF3888EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6B4C7B-6C54-6E4A-B6BB-1B3BD352D9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4369,6 +4369,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="31.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">

</xml_diff>